<commit_message>
Resolve merge conflict in add_record.py
</commit_message>
<xml_diff>
--- a/form_b_database.xlsx
+++ b/form_b_database.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,7 +468,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ffff</t>
+          <t>rrrrrrrrr</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -492,38 +492,6 @@
         </is>
       </c>
       <c r="F2" t="inlineStr">
-        <is>
-          <t>rff</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>eeeeeeeee</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>लक्ष्मीनगर</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>234</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
         <is>
           <t>rff</t>
         </is>

</xml_diff>